<commit_message>
RT lab 28 not finished yet. No theoretical evaluations.
</commit_message>
<xml_diff>
--- a/Radiotechnics_Labs/6_sem/Lab28/РТ лаба.xlsx
+++ b/Radiotechnics_Labs/6_sem/Lab28/РТ лаба.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexn\Documents\GitHub\Labs\Radiotechnics_Labs\6_sem\Lab28\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b566d95faa460c8a/GitHub/Labs/Radiotechnics_Labs/6_sem/Lab28/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C57B16-383D-4762-81D3-53F36023FF2A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="186" documentId="13_ncr:1_{C4C57B16-383D-4762-81D3-53F36023FF2A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{BAF1B57C-04EB-4BEC-BBFC-27A06599620B}"/>
   <bookViews>
-    <workbookView xWindow="4748" yWindow="712" windowWidth="17512" windowHeight="13598" xr2:uid="{B5517199-182B-4526-9411-7A2CEC385A30}"/>
+    <workbookView xWindow="-8400" yWindow="5460" windowWidth="17513" windowHeight="13598" activeTab="1" xr2:uid="{B5517199-182B-4526-9411-7A2CEC385A30}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Данные об авторе" sheetId="2" r:id="rId1"/>
+    <sheet name="Эксперимент" sheetId="1" r:id="rId2"/>
+    <sheet name="Теория" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
-  <si>
-    <t>Uk</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="39">
   <si>
     <t>Uб</t>
   </si>
@@ -54,9 +53,6 @@
     <t>Эксперимент 3</t>
   </si>
   <si>
-    <t>Uвых_макс</t>
-  </si>
-  <si>
     <t>В</t>
   </si>
   <si>
@@ -75,30 +71,18 @@
     <t>Uкэ</t>
   </si>
   <si>
-    <t>Найдем граничную частоту - ту, где нпряжние падает в sqrt(2) раз</t>
-  </si>
-  <si>
     <t>Iк</t>
   </si>
   <si>
-    <t>R</t>
-  </si>
-  <si>
     <t>кОм</t>
   </si>
   <si>
     <t>Uп</t>
   </si>
   <si>
-    <t>2 мА</t>
-  </si>
-  <si>
     <t>h21e</t>
   </si>
   <si>
-    <t>Эксперимент 2</t>
-  </si>
-  <si>
     <t>Uк</t>
   </si>
   <si>
@@ -109,12 +93,72 @@
   </si>
   <si>
     <t>Uвых макс</t>
+  </si>
+  <si>
+    <t>мА</t>
+  </si>
+  <si>
+    <t>Ток РК</t>
+  </si>
+  <si>
+    <t>Ток базы</t>
+  </si>
+  <si>
+    <t>Rк</t>
+  </si>
+  <si>
+    <t>Полученные значения</t>
+  </si>
+  <si>
+    <t>Rб</t>
+  </si>
+  <si>
+    <t>Параметры установки</t>
+  </si>
+  <si>
+    <t>Результаты</t>
+  </si>
+  <si>
+    <t>Rвх</t>
+  </si>
+  <si>
+    <t>Имя</t>
+  </si>
+  <si>
+    <t>Фамилия</t>
+  </si>
+  <si>
+    <t>Нехаев</t>
+  </si>
+  <si>
+    <t>Александр</t>
+  </si>
+  <si>
+    <t>Создание отчета автоматизировано.</t>
+  </si>
+  <si>
+    <t>Рыжие клетки - названия значений. Белые клетки - клетки предусматривающие ввод значений. В бледно-синих клетках содержатся рассчтанные значения.</t>
+  </si>
+  <si>
+    <t>Внимание! Проверяйте размерности в серых клетках (их менять нельзя).</t>
+  </si>
+  <si>
+    <t>Rи</t>
+  </si>
+  <si>
+    <t>Эксперимент 2б</t>
+  </si>
+  <si>
+    <t>Эксперимент 2а</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -125,12 +169,48 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -145,8 +225,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -460,263 +548,551 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{803B9F7F-1056-41BE-B881-EF152198F2A2}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AC762AF-F6C5-44B6-A995-C48304F3FE2E}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="1" max="1" width="13.46484375" customWidth="1"/>
     <col min="2" max="2" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>0.66</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3">
+        <v>620</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="5">
+        <f>(E4-B4)/(E5*1000)</f>
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="B4">
+        <v>5.2</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="5">
+        <f>(E4-B3)/(E3*1000)</f>
+        <v>1.5064516129032257E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2">
-        <v>0.66</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5">
+        <v>2.4</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="8">
+        <f>H3/H4</f>
+        <v>132.76231263383298</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="E2">
-        <v>620</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3">
-        <v>5.2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>76</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>180</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>22</v>
       </c>
       <c r="B9">
         <v>3.5</v>
       </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>23</v>
+      <c r="C9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="8">
+        <f>B9/(B10/1000)</f>
+        <v>152.17391304347825</v>
+      </c>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="B10">
         <v>23</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10">
+        <v>620</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="5">
+        <f>B9/(E9/1000)</f>
+        <v>70</v>
+      </c>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>76</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="8">
+        <f>(E5*1000*(B10/1000/((E9/1000)-(B10/1000))))/1000</f>
+        <v>2.0444444444444443</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>180</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>4.5</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>3.5</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>50</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="8">
+        <f>B17/(B18/1000)</f>
+        <v>152.17391304347825</v>
+      </c>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>23</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18">
+        <f>E10*2</f>
+        <v>1240</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="5">
+        <f>B17/(E17/1000)</f>
+        <v>70</v>
+      </c>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>76</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H19" s="8">
+        <f>(E5*1000*(B18/1000/((E17/1000)-(B18/1000))))/1000</f>
+        <v>2.0444444444444443</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>180</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>4.5</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A24" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E10">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25">
+        <v>80</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25">
         <v>50</v>
       </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12">
-        <v>76</v>
-      </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12">
-        <v>4.5</v>
-      </c>
-      <c r="F12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+      <c r="F25" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B13">
-        <v>180</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+      <c r="G25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="7">
+        <f>(B25/1000)/(B26/1000)</f>
+        <v>4.507042253521127</v>
+      </c>
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A26" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B16">
-        <v>80</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17">
+      <c r="B26">
         <f>35.5/2</f>
         <v>17.75</v>
       </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+      <c r="C26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26">
+        <v>2.4</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" s="7">
+        <f>(B25/1000)/(E25/1000)</f>
+        <v>1.5999999999999999</v>
+      </c>
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B18">
-        <v>0.05</v>
-      </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19">
+      <c r="B27">
         <v>85</v>
       </c>
-      <c r="C19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19">
+      <c r="C27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27">
         <f>35.5*0.7</f>
         <v>24.849999999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20">
+      <c r="G27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H27" s="7">
+        <f>(E5*1000*(B26/1000/((E25/1000)-(B26/1000))))/1000</f>
+        <v>1.3209302325581396</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28">
         <v>203</v>
       </c>
-      <c r="C20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21">
+      <c r="C28" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29">
         <f>330*5</f>
         <v>1650</v>
       </c>
-      <c r="C21" t="s">
-        <v>5</v>
+      <c r="C29" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46A4C0A4-CB39-400E-820B-A79ED3DB842D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
RT Lab updated, Lab 16 SSE report added.
</commit_message>
<xml_diff>
--- a/Radiotechnics_Labs/6_sem/Lab28/РТ лаба.xlsx
+++ b/Radiotechnics_Labs/6_sem/Lab28/РТ лаба.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexn\OneDrive\GitHub\Labs\Radiotechnics_Labs\6_sem\Lab28\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b566d95faa460c8a/GitHub/Labs/Radiotechnics_Labs/6_sem/Lab28/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="301" documentId="13_ncr:1_{C4C57B16-383D-4762-81D3-53F36023FF2A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{A91D2020-14DC-483C-8A52-C0EFD736CFE9}"/>
+  <xr:revisionPtr revIDLastSave="302" documentId="13_ncr:1_{C4C57B16-383D-4762-81D3-53F36023FF2A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{577E352E-4F13-4D8C-B39C-3FC120B5E763}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" activeTab="1" xr2:uid="{B5517199-182B-4526-9411-7A2CEC385A30}"/>
+    <workbookView xWindow="4770" yWindow="743" windowWidth="17512" windowHeight="13597" activeTab="1" xr2:uid="{B5517199-182B-4526-9411-7A2CEC385A30}"/>
   </bookViews>
   <sheets>
     <sheet name="Данные об авторе" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="54">
   <si>
     <t>Uб</t>
   </si>
@@ -883,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AC762AF-F6C5-44B6-A995-C48304F3FE2E}">
   <dimension ref="A1:W37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Z36" sqref="Z36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>